<commit_message>
added stemming related notebook and codes, generated stemmed movie term vector
</commit_message>
<xml_diff>
--- a/Documents/Profiling Approaches.xlsx
+++ b/Documents/Profiling Approaches.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
   <si>
     <t xml:space="preserve">Genre Profiles</t>
   </si>
@@ -448,6 +448,10 @@
     <t xml:space="preserve">For User U1</t>
   </si>
   <si>
+    <t xml:space="preserve">Movies in
+Final List</t>
+  </si>
+  <si>
     <t xml:space="preserve">Candidate Movie ID</t>
   </si>
   <si>
@@ -473,7 +477,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">c(u) | m &lt;?&gt;in&lt;?&gt; M</t>
+      <t xml:space="preserve">c(u) | m ϵ M</t>
     </r>
   </si>
   <si>
@@ -546,6 +550,31 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Cluster
+Score
+C</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">i</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Composite
 Score</t>
   </si>
@@ -554,13 +583,266 @@
 Rank</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m1</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(M1)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">M10</t>
   </si>
   <si>
+    <t xml:space="preserve">No of movies</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Cluster Rank
+RN</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Score(SC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
+=
+(#C – RN</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m1</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(M2)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[M10]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m2</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(M3)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">M11</t>
   </si>
   <si>
+    <t xml:space="preserve">[M11, M12]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m2</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(M4)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[M31, M32, M33, M34, M35, M36, M37, M38]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m2</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(M5)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">M12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[M41, M42, M43, M44, M45, M46, M47, M48, M49]</t>
   </si>
   <si>
     <t xml:space="preserve">Deliverable Results</t>
@@ -616,7 +898,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -681,6 +963,13 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FFEEEEEE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -789,7 +1078,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -928,6 +1217,22 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1279,7 +1584,7 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1497,7 +1802,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.69"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.81"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.39"/>
@@ -2169,10 +2474,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2181,14 +2486,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="3.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="36.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="46.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="65.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="43.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2203,6 +2509,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
@@ -2216,6 +2523,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -2234,13 +2542,14 @@
       <c r="F3" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2263,13 +2572,14 @@
         <f aca="false">30/100</f>
         <v>0.3</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="n">
         <f aca="false">20/100</f>
         <v>0.2</v>
       </c>
-      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="K4" s="11" t="s">
+      <c r="J4" s="1"/>
+      <c r="L4" s="11" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2291,7 +2601,8 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="L5" s="11" t="s">
+      <c r="J5" s="1"/>
+      <c r="M5" s="11" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2313,7 +2624,8 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="M6" s="33" t="s">
+      <c r="J6" s="1"/>
+      <c r="N6" s="33" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2335,6 +2647,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
@@ -2348,7 +2661,8 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="L8" s="11" t="s">
+      <c r="J8" s="1"/>
+      <c r="M8" s="11" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2364,7 +2678,8 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="M9" s="33" t="s">
+      <c r="J9" s="1"/>
+      <c r="N9" s="33" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2380,6 +2695,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
@@ -2393,7 +2709,8 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="L11" s="9" t="s">
+      <c r="J11" s="1"/>
+      <c r="M11" s="9" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2407,7 +2724,8 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="M12" s="33" t="s">
+      <c r="J12" s="1"/>
+      <c r="N12" s="33" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2429,39 +2747,48 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="48.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>107</v>
+      <c r="A18" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" s="34" t="s">
         <v>113</v>
       </c>
+      <c r="G18" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="H18" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>115</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C19" s="5" t="n">
         <v>4.5</v>
@@ -2476,19 +2803,37 @@
         <v>0.7</v>
       </c>
       <c r="G19" s="1" t="n">
-        <f aca="false"> C19 * D19 * E19*F19</f>
-        <v>0.756</v>
+        <v>4</v>
       </c>
       <c r="H19" s="1" t="n">
+        <f aca="false">C19 * D19 * E19*F19*G19</f>
+        <v>3.024</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" s="35" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="N19" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="O19" s="36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>4.5</v>
@@ -2503,19 +2848,37 @@
         <v>0.65</v>
       </c>
       <c r="G20" s="1" t="n">
-        <f aca="false"> C20 * D20 * E20*F20</f>
-        <v>0.702</v>
+        <v>4</v>
       </c>
       <c r="H20" s="1" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">C20 * D20 * E20*F20*G20</f>
+        <v>2.808</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K20" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="M20" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" s="37" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>12</v>
+        <v>124</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>4.2</v>
@@ -2530,19 +2893,37 @@
         <v>0.8</v>
       </c>
       <c r="G21" s="1" t="n">
-        <f aca="false"> C21 * D21 * E21*F21</f>
-        <v>0.783216</v>
+        <v>3</v>
       </c>
       <c r="H21" s="1" t="n">
+        <f aca="false">C21 * D21 * E21*F21*G21</f>
+        <v>2.349648</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K21" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="L21" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="M21" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="N21" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="O21" s="37" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>4.2</v>
@@ -2557,19 +2938,37 @@
         <v>0.85</v>
       </c>
       <c r="G22" s="1" t="n">
-        <f aca="false"> C22 * D22 * E22*F22</f>
-        <v>0.832167</v>
+        <v>3</v>
       </c>
       <c r="H22" s="1" t="n">
+        <f aca="false">C22 * D22 * E22*F22*G22</f>
+        <v>2.496501</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="K22" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="L22" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="M22" s="35" t="n">
+        <v>8</v>
+      </c>
+      <c r="N22" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="O22" s="35" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>14</v>
+        <v>129</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>4.6</v>
@@ -2584,17 +2983,35 @@
         <v>0.95</v>
       </c>
       <c r="G23" s="1" t="n">
-        <f aca="false"> C23 * D23 * E23*F23</f>
-        <v>0.994175</v>
+        <v>3</v>
       </c>
       <c r="H23" s="1" t="n">
+        <f aca="false">C23 * D23 * E23*F23*G23</f>
+        <v>2.982525</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K23" s="35" t="n">
+        <v>4</v>
+      </c>
+      <c r="L23" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="M23" s="35" t="n">
+        <v>9</v>
+      </c>
+      <c r="N23" s="35" t="n">
+        <v>4</v>
+      </c>
+      <c r="O23" s="35" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="D2:J2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -2631,37 +3048,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="11" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
@@ -2670,10 +3087,10 @@
         <v>3</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2681,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2689,7 +3106,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,7 +3114,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,7 +3122,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2713,7 +3130,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tracker, added evaluation metrics, and more reference docs
</commit_message>
<xml_diff>
--- a/Documents/Profiling Approaches.xlsx
+++ b/Documents/Profiling Approaches.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="141">
   <si>
     <t xml:space="preserve">Genre Profiles</t>
   </si>
@@ -405,47 +405,16 @@
     <t xml:space="preserve">The weight to consider along with this frequency is ‘Movie Count Based Mean’</t>
   </si>
   <si>
-    <t xml:space="preserve">t1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t6</t>
-  </si>
-  <si>
     <t xml:space="preserve">For each movie in recommendation list</t>
   </si>
   <si>
     <t xml:space="preserve">S_u = find similarity with user’s profile</t>
   </si>
   <si>
+    <t xml:space="preserve">For User U1</t>
+  </si>
+  <si>
     <t xml:space="preserve">TODO define user’s profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversity = 1 – similarity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TODO use this definition to calculate diversity or use std def’s from literature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S_c = (average in case of multiple candidate movies)
-Similarity to candidate movie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TODO verify formula for divesity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For User U1</t>
   </si>
   <si>
     <t xml:space="preserve">Movies in
@@ -619,6 +588,157 @@
     <t xml:space="preserve">M10</t>
   </si>
   <si>
+    <t xml:space="preserve">Diversity = 1 – similarity</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m1</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(M2)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO use this definition to calculate diversity or use std def’s from literature</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m2</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(M3)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">M11</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m2</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(M4)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">S_c = (average in case of multiple candidate movies)
+Similarity to candidate movie</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m2</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(M5)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">M12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO verify formula for divesity</t>
+  </si>
+  <si>
     <t xml:space="preserve">No of movies</t>
   </si>
   <si>
@@ -695,151 +815,13 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">m1</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(M2)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">[M10]</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">m2</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(M3)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">M11</t>
-  </si>
-  <si>
     <t xml:space="preserve">[M11, M12]</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">m2</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(M4)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">[M31, M32, M33, M34, M35, M36, M37, M38]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">m2</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(M5)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">M12</t>
   </si>
   <si>
     <t xml:space="preserve">[M41, M42, M43, M44, M45, M46, M47, M48, M49]</t>
@@ -2474,36 +2456,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="5.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.69"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="43.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="36.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="36.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="65.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2515,9 +2497,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -2526,485 +2506,347 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>96</v>
-      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>99</v>
-      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="n">
-        <f aca="false">2/100</f>
-        <v>0.02</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <f aca="false">30/100</f>
-        <v>0.3</v>
-      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1" t="n">
-        <f aca="false">20/100</f>
-        <v>0.2</v>
-      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="L4" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="M5" s="11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="B6" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="N6" s="33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="79.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="B8" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <f aca="false">D8 * E8 * F8*G8*H8</f>
+        <v>3.024</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="M8" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="B9" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <f aca="false">D9 * E9 * F9*G9*H9</f>
+        <v>2.808</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="N9" s="33" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <f aca="false">D10 * E10 * F10*G10*H10</f>
+        <v>2.349648</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="B11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <f aca="false">D11 * E11 * F11*G11*H11</f>
+        <v>2.496501</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="M11" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="B12" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <f aca="false">D12 * E12 * F12*G12*H12</f>
+        <v>2.982525</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="N12" s="33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>18</v>
-      </c>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>4</v>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
+    <row r="16" customFormat="false" ht="84.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>121</v>
+      </c>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="48.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H18" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="5" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="F19" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="G19" s="1" t="n">
+      <c r="B17" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="37" t="n">
         <v>4</v>
       </c>
-      <c r="H19" s="1" t="n">
-        <f aca="false">C19 * D19 * E19*F19*G19</f>
-        <v>3.024</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K19" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="L19" s="35" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="37" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="35" t="n">
+        <v>8</v>
+      </c>
+      <c r="E19" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" s="35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="M19" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="N19" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="O19" s="36" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="F20" s="1" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="G20" s="1" t="n">
+      <c r="C20" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="35" t="n">
+        <v>9</v>
+      </c>
+      <c r="E20" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="H20" s="1" t="n">
-        <f aca="false">C20 * D20 * E20*F20*G20</f>
-        <v>2.808</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K20" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="L20" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="M20" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="N20" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="O20" s="37" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="F21" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <f aca="false">C21 * D21 * E21*F21*G21</f>
-        <v>2.349648</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="K21" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="L21" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="M21" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="N21" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="O21" s="37" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="E22" s="1" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="F22" s="1" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <f aca="false">C22 * D22 * E22*F22*G22</f>
-        <v>2.496501</v>
-      </c>
-      <c r="I22" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="K22" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="L22" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="M22" s="35" t="n">
-        <v>8</v>
-      </c>
-      <c r="N22" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="O22" s="35" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="F23" s="1" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <f aca="false">C23 * D23 * E23*F23*G23</f>
-        <v>2.982525</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K23" s="35" t="n">
-        <v>4</v>
-      </c>
-      <c r="L23" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="M23" s="35" t="n">
-        <v>9</v>
-      </c>
-      <c r="N23" s="35" t="n">
-        <v>4</v>
-      </c>
-      <c r="O23" s="35" t="n">
+      <c r="F20" s="35" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3048,37 +2890,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="11" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
@@ -3087,10 +2929,10 @@
         <v>3</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3098,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3106,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3114,7 +2956,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3122,7 +2964,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3130,7 +2972,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated cluster targetting and ranking
</commit_message>
<xml_diff>
--- a/Documents/Profiling Approaches.xlsx
+++ b/Documents/Profiling Approaches.xlsx
@@ -744,6 +744,7 @@
   <si>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -754,6 +755,7 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
         <vertAlign val="subscript"/>
         <sz val="10"/>
         <rFont val="Arial"/>
@@ -766,6 +768,7 @@
   <si>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -775,6 +778,7 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
         <vertAlign val="subscript"/>
         <sz val="10"/>
         <rFont val="Arial"/>
@@ -785,6 +789,7 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -796,6 +801,7 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
         <vertAlign val="subscript"/>
         <sz val="10"/>
         <rFont val="Arial"/>
@@ -806,6 +812,7 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -880,7 +887,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -945,13 +952,6 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FFEEEEEE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1060,7 +1060,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1201,19 +1201,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2459,19 +2455,19 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.69"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
@@ -2765,88 +2761,88 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="84.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="35" t="s">
+    <row r="16" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="8" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="37" t="s">
+      <c r="B17" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="37" t="n">
+      <c r="D17" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="35" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="37" t="n">
+      <c r="B18" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="37" t="n">
+      <c r="D18" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="E18" s="37" t="n">
+      <c r="E18" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="F18" s="37" t="n">
+      <c r="F18" s="35" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="35" t="n">
+      <c r="B19" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="D19" s="35" t="n">
+      <c r="D19" s="37" t="n">
         <v>8</v>
       </c>
-      <c r="E19" s="35" t="n">
+      <c r="E19" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="F19" s="35" t="n">
+      <c r="F19" s="37" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="35" t="n">
+      <c r="B20" s="37" t="n">
         <v>4</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="35" t="n">
+      <c r="D20" s="37" t="n">
         <v>9</v>
       </c>
-      <c r="E20" s="35" t="n">
+      <c r="E20" s="37" t="n">
         <v>4</v>
       </c>
-      <c r="F20" s="35" t="n">
+      <c r="F20" s="37" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>